<commit_message>
add asm to ignore
</commit_message>
<xml_diff>
--- a/versions/rank.xlsx
+++ b/versions/rank.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>version</t>
   </si>
@@ -45,19 +45,22 @@
   <si>
     <t>inline-regbug</t>
   </si>
+  <si>
+    <t>no redundant regload</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +81,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10.5"/>
+      <color rgb="FF333333"/>
+      <name val="Lucida Console"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
@@ -86,21 +95,75 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -108,53 +171,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -184,10 +200,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -209,14 +225,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,181 +252,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,6 +458,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -464,17 +497,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -496,18 +523,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -526,27 +546,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -555,137 +564,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -698,25 +707,28 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1037,13 +1049,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="1" width="16.3333333333333" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.3333333333333" style="2" customWidth="1"/>
@@ -1172,7 +1184,7 @@
         <v>517265.5</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" ht="14.75" spans="1:13">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -1211,6 +1223,47 @@
       </c>
       <c r="M4" s="8">
         <v>517265.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="12">
+        <v>2522610</v>
+      </c>
+      <c r="C5" s="12">
+        <v>2522610</v>
+      </c>
+      <c r="D5" s="12">
+        <v>4802121</v>
+      </c>
+      <c r="E5" s="12">
+        <v>4802121</v>
+      </c>
+      <c r="F5" s="12">
+        <v>279823039.5</v>
+      </c>
+      <c r="G5" s="12">
+        <v>279823039.5</v>
+      </c>
+      <c r="H5" s="12">
+        <v>596386.5</v>
+      </c>
+      <c r="I5" s="12">
+        <v>596386.5</v>
+      </c>
+      <c r="J5" s="12">
+        <v>1009063.5</v>
+      </c>
+      <c r="K5" s="12">
+        <v>1009063.5</v>
+      </c>
+      <c r="L5" s="12">
+        <v>513256</v>
+      </c>
+      <c r="M5" s="12">
+        <v>513256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish dce and div-mod
</commit_message>
<xml_diff>
--- a/versions/rank.xlsx
+++ b/versions/rank.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>version</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t>daG</t>
+  </si>
+  <si>
+    <t>one-time-comm-dce</t>
+  </si>
+  <si>
+    <t>10 times comm dce</t>
+  </si>
+  <si>
+    <t>div mod</t>
   </si>
 </sst>
 </file>
@@ -64,10 +73,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -102,6 +111,44 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -110,92 +157,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -207,9 +171,63 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -223,17 +241,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -246,7 +255,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,199 +264,205 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF5F5F5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,6 +482,30 @@
         <color rgb="FFDDDDDD"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -488,8 +527,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -509,6 +548,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -520,39 +568,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -573,10 +588,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -585,7 +600,7 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -594,150 +609,152 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -746,21 +763,36 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1082,13 +1114,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="16.3333333333333" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.3333333333333" style="2" customWidth="1"/>
@@ -1258,44 +1290,44 @@
         <v>517265.5</v>
       </c>
     </row>
-    <row r="5" ht="14.75" spans="1:13">
+    <row r="5" ht="28.75" spans="1:13">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="12">
         <v>2522610</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="13">
         <v>2522610</v>
       </c>
       <c r="D5" s="12">
         <v>4802121</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="13">
         <v>4802121</v>
       </c>
       <c r="F5" s="12">
         <v>279823039.5</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="14">
         <v>279823039.5</v>
       </c>
       <c r="H5" s="12">
         <v>596386.5</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="13">
         <v>596386.5</v>
       </c>
       <c r="J5" s="12">
         <v>1009063.5</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="13">
         <v>1009063.5</v>
       </c>
       <c r="L5" s="12">
         <v>513256</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="13">
         <v>513256</v>
       </c>
     </row>
@@ -1303,40 +1335,40 @@
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="15">
         <v>2421112.5</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="16">
         <v>2421112.5</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="15">
         <v>4798871</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="16">
         <v>4798871</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="15">
         <v>261658564</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="16">
         <v>261658564</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="15">
         <v>581222.5</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="16">
         <v>581222.5</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="15">
         <v>998683.5</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="16">
         <v>998683.5</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="15">
         <v>479755</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="16">
         <v>479755</v>
       </c>
     </row>
@@ -1344,81 +1376,204 @@
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="17">
         <v>2202351.5</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="16">
         <v>2202351.5</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="17">
         <v>4740853</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="16">
         <v>4740853</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="17">
         <v>215500815</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="16">
         <v>215500815</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="17">
         <v>424182.5</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="16">
         <v>424182.5</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="17">
         <v>797614.5</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="16">
         <v>797614.5</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="17">
         <v>368521</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="16">
         <v>368521</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" ht="14.75" spans="1:13">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="15">
         <v>2436617</v>
       </c>
       <c r="C8" s="16">
         <v>2202351.5</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="15">
         <v>6490854</v>
       </c>
       <c r="E8" s="16">
         <v>4740853</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="15">
         <v>230632426</v>
       </c>
       <c r="G8" s="16">
         <v>215500815</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="15">
         <v>427275</v>
       </c>
       <c r="I8" s="16">
         <v>424182.5</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="20">
         <v>832929.5</v>
       </c>
       <c r="K8" s="16">
         <v>797614.5</v>
       </c>
-      <c r="L8" s="16">
+      <c r="L8" s="15">
         <v>389516</v>
       </c>
       <c r="M8" s="16">
+        <v>368521</v>
+      </c>
+    </row>
+    <row r="9" ht="28.75" spans="1:13">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="17">
+        <v>2436344</v>
+      </c>
+      <c r="C9" s="16">
+        <v>2202351.5</v>
+      </c>
+      <c r="D9" s="17">
+        <v>6489104</v>
+      </c>
+      <c r="E9" s="16">
+        <v>4740853</v>
+      </c>
+      <c r="F9" s="17">
+        <v>230632273.5</v>
+      </c>
+      <c r="G9" s="16">
+        <v>215500815</v>
+      </c>
+      <c r="H9" s="17">
+        <v>427275</v>
+      </c>
+      <c r="I9" s="16">
+        <v>424182.5</v>
+      </c>
+      <c r="J9" s="17">
+        <v>818275</v>
+      </c>
+      <c r="K9" s="16">
+        <v>797614.5</v>
+      </c>
+      <c r="L9" s="21">
+        <v>381837.5</v>
+      </c>
+      <c r="M9" s="16">
+        <v>368521</v>
+      </c>
+    </row>
+    <row r="10" ht="28.75" spans="1:13">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="15">
+        <v>2436296</v>
+      </c>
+      <c r="C10" s="16">
+        <v>2202351.5</v>
+      </c>
+      <c r="D10" s="15">
+        <v>6489104</v>
+      </c>
+      <c r="E10" s="16">
+        <v>4740853</v>
+      </c>
+      <c r="F10" s="15">
+        <v>230632174.5</v>
+      </c>
+      <c r="G10" s="16">
+        <v>215500815</v>
+      </c>
+      <c r="H10" s="15">
+        <v>427275</v>
+      </c>
+      <c r="I10" s="16">
+        <v>424182.5</v>
+      </c>
+      <c r="J10" s="15">
+        <v>818275</v>
+      </c>
+      <c r="K10" s="16">
+        <v>797614.5</v>
+      </c>
+      <c r="L10" s="15">
+        <v>374595.5</v>
+      </c>
+      <c r="M10" s="16">
+        <v>368521</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2436329</v>
+      </c>
+      <c r="C11" s="19">
+        <v>2202351.5</v>
+      </c>
+      <c r="D11" s="18">
+        <v>6490853</v>
+      </c>
+      <c r="E11" s="19">
+        <v>4740853</v>
+      </c>
+      <c r="F11" s="18">
+        <v>122941217.5</v>
+      </c>
+      <c r="G11" s="19">
+        <v>122941217.5</v>
+      </c>
+      <c r="H11" s="18">
+        <v>427275</v>
+      </c>
+      <c r="I11" s="19">
+        <v>424182.5</v>
+      </c>
+      <c r="J11" s="18">
+        <v>823993.5</v>
+      </c>
+      <c r="K11" s="19">
+        <v>797614.5</v>
+      </c>
+      <c r="L11" s="18">
+        <v>387828</v>
+      </c>
+      <c r="M11" s="19">
         <v>368521</v>
       </c>
     </row>

</xml_diff>

<commit_message>
delete a unless loop in main
</commit_message>
<xml_diff>
--- a/versions/rank.xlsx
+++ b/versions/rank.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>version</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>div mod</t>
+  </si>
+  <si>
+    <t>mod</t>
   </si>
 </sst>
 </file>
@@ -73,9 +76,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
   <fonts count="24">
@@ -111,6 +114,97 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -119,8 +213,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -128,116 +223,24 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -282,13 +285,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -300,169 +423,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,9 +490,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -509,17 +529,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -529,30 +543,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -574,11 +564,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -588,10 +591,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -600,137 +603,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -783,16 +786,13 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1114,10 +1114,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1488,7 +1488,7 @@
       <c r="K9" s="16">
         <v>797614.5</v>
       </c>
-      <c r="L9" s="21">
+      <c r="L9" s="18">
         <v>381837.5</v>
       </c>
       <c r="M9" s="16">
@@ -1536,20 +1536,20 @@
         <v>368521</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" ht="14.75" spans="1:13">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="17">
         <v>2436329</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="16">
         <v>2202351.5</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>6490853</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="16">
         <v>4740853</v>
       </c>
       <c r="F11" s="18">
@@ -1558,23 +1558,64 @@
       <c r="G11" s="19">
         <v>122941217.5</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="17">
         <v>427275</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="16">
         <v>424182.5</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="17">
         <v>823993.5</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="16">
         <v>797614.5</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="17">
         <v>387828</v>
       </c>
-      <c r="M11" s="19">
+      <c r="M11" s="16">
         <v>368521</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="17">
+        <v>2202068.5</v>
+      </c>
+      <c r="C12" s="17">
+        <v>2202068.5</v>
+      </c>
+      <c r="D12" s="17">
+        <v>4739104</v>
+      </c>
+      <c r="E12" s="17">
+        <v>4739104</v>
+      </c>
+      <c r="F12" s="17">
+        <v>110231674.5</v>
+      </c>
+      <c r="G12" s="17">
+        <v>107810815</v>
+      </c>
+      <c r="H12" s="17">
+        <v>423932.5</v>
+      </c>
+      <c r="I12" s="17">
+        <v>423932.5</v>
+      </c>
+      <c r="J12" s="17">
+        <v>784689.5</v>
+      </c>
+      <c r="K12" s="17">
+        <v>784689.5</v>
+      </c>
+      <c r="L12" s="17">
+        <v>346793.5</v>
+      </c>
+      <c r="M12" s="17">
+        <v>346793.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>